<commit_message>
Modify inflicts with teaching calendar
</commit_message>
<xml_diff>
--- a/IAEA/值班表/ITF-小学期空课表.xlsx
+++ b/IAEA/值班表/ITF-小学期空课表.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\ITF\IAEA\值班表\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE41F83-62A3-4E8A-9E32-C707DFA245C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C267B866-540D-40A2-854A-8C04844A7BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="593" yWindow="1740" windowWidth="17070" windowHeight="9540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -587,7 +587,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -639,7 +639,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>18</v>
@@ -648,7 +648,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>16</v>
@@ -660,7 +660,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>18</v>
@@ -669,7 +669,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>16</v>

</xml_diff>